<commit_message>
Added power options to the arduino side
</commit_message>
<xml_diff>
--- a/PID_Controller/i2c_registries.xlsx
+++ b/PID_Controller/i2c_registries.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="976" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>I2C Registry</t>
   </si>
@@ -49,7 +49,7 @@
     <t>pitch decimal number</t>
   </si>
   <si>
-    <t>motor 4 </t>
+    <t>motor 4</t>
   </si>
   <si>
     <t>roll whole number</t>
@@ -67,6 +67,9 @@
     <t>update kp</t>
   </si>
   <si>
+    <t>read killswitch state</t>
+  </si>
+  <si>
     <t>update ki</t>
   </si>
   <si>
@@ -77,6 +80,18 @@
   </si>
   <si>
     <t>update desired depth</t>
+  </si>
+  <si>
+    <t>Update desired pitch</t>
+  </si>
+  <si>
+    <t>Update desired roll</t>
+  </si>
+  <si>
+    <t>Update throttle Default 0</t>
+  </si>
+  <si>
+    <t>enable or disable power to motors</t>
   </si>
 </sst>
 </file>
@@ -245,10 +260,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -363,13 +378,19 @@
       <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="D8" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -377,7 +398,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -385,7 +406,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -393,7 +414,39 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>